<commit_message>
Fix multiple imputation spaghetti plot
</commit_message>
<xml_diff>
--- a/OSI/Budget.xlsx
+++ b/OSI/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402DF8BB-D489-4192-A42B-07956EF277E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C78B8-AD80-425F-8716-BD39F591AABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11835" yWindow="4650" windowWidth="17070" windowHeight="14010" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">Gruppenavn: </t>
   </si>
@@ -308,16 +308,20 @@
   </si>
   <si>
     <t>Training fee refund (Ok Kyong)</t>
+  </si>
+  <si>
+    <t>Budsjett 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$kr-414]"/>
     <numFmt numFmtId="165" formatCode="&quot;kr &quot;#,##0.00;[Red]&quot;-kr &quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$kr-414]\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_-[$kr-414]\ * #,##0.00_-;\-[$kr-414]\ * #,##0.00_-;_-[$kr-414]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -383,7 +387,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +409,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,129 +480,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -938,1124 +963,1156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="31"/>
-    <col min="6" max="6" width="14.42578125" style="33"/>
-    <col min="7" max="16384" width="14.42578125" style="2"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="23"/>
+    <col min="6" max="6" width="14.42578125" style="25"/>
+    <col min="7" max="7" width="14.42578125" style="1"/>
+    <col min="8" max="8" width="14.42578125" style="43"/>
+    <col min="9" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2">
+      <c r="B2" s="34"/>
+      <c r="C2" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
+      <c r="H9" s="44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>3110</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="9">
         <f>7000</f>
         <v>7000</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="42">
         <v>2990</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="26">
         <f>E10-C10</f>
         <v>-4010</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+      <c r="H10" s="43">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
         <v>3120</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="34"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="C11" s="9"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>3400</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="34"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+      <c r="C12" s="9"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <v>3440</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="34"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
+      <c r="C13" s="9"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>3480</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="9">
         <f>C20</f>
         <v>20800</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="32">
+      <c r="D14" s="4"/>
+      <c r="E14" s="24">
         <v>1500</v>
       </c>
-      <c r="F14" s="34">
-        <f t="shared" ref="F11:F26" si="0">E14-C14</f>
+      <c r="F14" s="26">
+        <f t="shared" ref="F14:F26" si="0">E14-C14</f>
         <v>-19300</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12">
+      <c r="H14" s="43">
+        <v>20800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>3490</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="9">
         <f>50*38</f>
         <v>1900</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="24">
         <v>4600</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="26">
         <f t="shared" si="0"/>
         <v>2700</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12">
+      <c r="H15" s="43">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <v>3610</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="34"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12">
+      <c r="C16" s="9"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>3630</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="34"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12">
+      <c r="C17" s="9"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="26"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
         <v>3900</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="34"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12">
+      <c r="C18" s="9"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <v>3910</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="34"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12">
+      <c r="C19" s="9"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
         <v>3920</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="9">
         <f>10*590*2+50*90*2</f>
         <v>20800</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="42">
         <v>12880</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="26">
         <f t="shared" si="0"/>
         <v>-7920</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12">
+      <c r="H20" s="43">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
         <v>3940</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="34"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
+      <c r="C21" s="9"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
         <v>3950</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="34"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
+      <c r="C22" s="9"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>3960</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="34"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
+      <c r="C23" s="9"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="26"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
         <v>3970</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="34"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="15">
+      <c r="C24" s="9"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="26"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
         <v>3990</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="34"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19">
+      <c r="B26" s="39"/>
+      <c r="C26" s="13">
         <f>SUM(C10:C25)</f>
         <v>50500</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="37">
+      <c r="D26" s="4"/>
+      <c r="E26" s="29">
         <f>SUM(E10:E25)</f>
         <v>21970</v>
       </c>
-      <c r="F26" s="38">
+      <c r="F26" s="30">
         <f t="shared" si="0"/>
         <v>-28530</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="34"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="34"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="12">
+      <c r="B28" s="40"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="26"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
         <v>5010</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="34"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="12">
+      <c r="C29" s="9"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
         <v>5011</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="34"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="12">
+      <c r="C30" s="9"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
         <v>5020</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="34"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="12">
+      <c r="C31" s="9"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
         <v>5250</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="34"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="12">
+      <c r="A33" s="7">
         <v>5350</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="34"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="15">
+      <c r="A34" s="10">
         <v>5990</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="34"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="26"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24">
+      <c r="B35" s="41"/>
+      <c r="C35" s="16">
         <f>SUM(C29:C34)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="34"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="26"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="34"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="34"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="12">
+      <c r="A38" s="7">
         <v>4110</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="9">
         <v>9065</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="32">
+      <c r="D38" s="4"/>
+      <c r="E38" s="24">
         <v>0</v>
       </c>
-      <c r="F38" s="34">
+      <c r="F38" s="26">
         <f>E38-C38</f>
         <v>-9065</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="12">
+      <c r="A39" s="7">
         <v>4120</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="9">
         <v>3000</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="32">
-        <v>0</v>
-      </c>
-      <c r="F39" s="34">
+      <c r="D39" s="18"/>
+      <c r="E39" s="24">
+        <v>10599</v>
+      </c>
+      <c r="F39" s="26">
         <f>E39-C39</f>
-        <v>-3000</v>
+        <v>7599</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="12">
+      <c r="A40" s="7">
         <v>4150</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="34"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="26"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="12">
+      <c r="A41" s="7">
         <v>4200</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="9">
         <v>1000</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="32">
+      <c r="E41" s="24">
         <v>9100</v>
       </c>
-      <c r="F41" s="34">
-        <f t="shared" ref="F40:F80" si="1">E41-C41</f>
+      <c r="F41" s="26">
+        <f t="shared" ref="F41:F78" si="1">E41-C41</f>
         <v>8100</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="22" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="12">
+      <c r="A42" s="7">
         <v>4300</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="34"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="12">
+      <c r="A43" s="7">
         <v>4500</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="34"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="12">
+      <c r="A44" s="7">
         <v>4510</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="34"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="26"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="12">
+      <c r="A45" s="7">
         <v>4610</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="34"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="26"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="12">
+      <c r="A46" s="7">
         <v>4700</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="34"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="26"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="12">
+      <c r="A47" s="7">
         <v>4800</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="9">
         <f>650*10*2</f>
         <v>13000</v>
       </c>
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="32">
+      <c r="E47" s="24">
         <v>616.75</v>
       </c>
-      <c r="F47" s="34">
+      <c r="F47" s="26">
         <f t="shared" si="1"/>
         <v>-12383.25</v>
       </c>
-      <c r="G47" s="30" t="s">
+      <c r="G47" s="22" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="12">
+      <c r="A48" s="7">
         <v>4990</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="9">
         <f>7500+7500</f>
         <v>15000</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="32">
+      <c r="D48" s="19"/>
+      <c r="E48" s="24">
         <v>4800.55</v>
       </c>
-      <c r="F48" s="34">
+      <c r="F48" s="26">
         <f t="shared" si="1"/>
         <v>-10199.450000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="12">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
         <v>6110</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="34"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="12">
+      <c r="C49" s="9"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="26"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
         <v>6300</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="34"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="12">
+      <c r="C50" s="9"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="26"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
         <v>6320</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="34"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="12">
+      <c r="C51" s="9"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="26"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
         <v>6340</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="34"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="12">
+      <c r="C52" s="9"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="26"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
         <v>6420</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="34"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="12">
+      <c r="C53" s="9"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="26"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
         <v>6440</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="34"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="12">
+      <c r="C54" s="9"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="26"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
         <v>6540</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="34"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="12">
+      <c r="C55" s="9"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="26"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
         <v>6550</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="34"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="12">
+      <c r="C56" s="9"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="26"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
         <v>6620</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="34"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="12">
+      <c r="C57" s="9"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="26"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
         <v>6700</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="34"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="12">
+      <c r="C58" s="9"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="26"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
         <v>6712</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="34"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="12">
+      <c r="C59" s="9"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="26"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
         <v>6730</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="34"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="12">
+      <c r="C60" s="9"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="26"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
         <v>6790</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="34"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="12">
+      <c r="C61" s="9"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="26"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
         <v>6800</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="34"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="12">
+      <c r="C62" s="9"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="26"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
         <v>6810</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="9">
         <v>85</v>
       </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="32">
+      <c r="D63" s="4"/>
+      <c r="E63" s="24">
         <v>0</v>
       </c>
-      <c r="F63" s="34">
+      <c r="F63" s="26">
         <f t="shared" si="1"/>
         <v>-85</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="12">
+      <c r="H63" s="43">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
         <v>6811</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C64" s="9">
         <v>136.25</v>
       </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="32">
+      <c r="D64" s="4"/>
+      <c r="E64" s="24">
         <v>0</v>
       </c>
-      <c r="F64" s="34">
+      <c r="F64" s="26">
         <f t="shared" si="1"/>
         <v>-136.25</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="12">
+      <c r="H64" s="43">
+        <v>136.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
         <v>6820</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C65" s="9">
         <v>1500</v>
       </c>
-      <c r="D65" s="26"/>
-      <c r="E65" s="32">
+      <c r="D65" s="18"/>
+      <c r="E65" s="24">
         <v>0</v>
       </c>
-      <c r="F65" s="34">
+      <c r="F65" s="26">
         <f t="shared" si="1"/>
         <v>-1500</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="12">
+      <c r="H65" s="43">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
         <v>6840</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66" s="9">
         <v>500</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="32">
+      <c r="E66" s="24">
         <v>1000</v>
       </c>
-      <c r="F66" s="34">
+      <c r="F66" s="26">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="12">
+      <c r="H66" s="43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
         <v>6860</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="9">
         <v>7000</v>
       </c>
-      <c r="D67" s="28"/>
-      <c r="E67" s="32">
+      <c r="D67" s="20"/>
+      <c r="E67" s="24">
         <v>1009.93</v>
       </c>
-      <c r="F67" s="34">
+      <c r="F67" s="26">
         <f t="shared" si="1"/>
         <v>-5990.07</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="12">
+      <c r="H67" s="43">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
         <v>6900</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="34"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="12">
+      <c r="C68" s="9"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="26"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
         <v>6940</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C69" s="14"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="34"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="12">
+      <c r="C69" s="9"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="26"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="7">
         <v>7100</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="34"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="12">
+      <c r="C70" s="9"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="26"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="7">
         <v>7110</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="14"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="34"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="12">
+      <c r="C71" s="9"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="26"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
         <v>7320</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="14"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="34"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="12">
+      <c r="C72" s="9"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="26"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
         <v>7420</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C73" s="14"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="34"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="12">
+      <c r="C73" s="9"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="26"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
         <v>7500</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C74" s="14"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="34"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="12">
+      <c r="C74" s="9"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="26"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="7">
         <v>7510</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C75" s="14"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="34"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="12">
+      <c r="C75" s="9"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="26"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
         <v>7700</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="34"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="15">
+      <c r="C76" s="9"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="26"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="10">
         <v>7790</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C77" s="17"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="34"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="23" t="s">
+      <c r="C77" s="12"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="26"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="23"/>
-      <c r="C78" s="19">
+      <c r="B78" s="41"/>
+      <c r="C78" s="13">
         <f>SUM(C38:C77)</f>
         <v>50286.25</v>
       </c>
-      <c r="D78" s="7"/>
-      <c r="E78" s="32">
+      <c r="D78" s="4"/>
+      <c r="E78" s="24">
         <f>SUM(E38:E77)</f>
-        <v>16527.23</v>
-      </c>
-      <c r="F78" s="34">
+        <v>27126.23</v>
+      </c>
+      <c r="F78" s="26">
         <f t="shared" si="1"/>
-        <v>-33759.020000000004</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="29"/>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="7"/>
-      <c r="F79" s="34"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="18" t="s">
+        <v>-23160.02</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="4"/>
+      <c r="F79" s="26"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19">
+      <c r="B80" s="39"/>
+      <c r="C80" s="13">
         <f>C78+C35</f>
         <v>50286.25</v>
       </c>
-      <c r="D80" s="7"/>
-      <c r="E80" s="39">
+      <c r="D80" s="4"/>
+      <c r="E80" s="31">
         <f>E78</f>
-        <v>16527.23</v>
-      </c>
-      <c r="F80" s="38">
+        <v>27126.23</v>
+      </c>
+      <c r="F80" s="30">
         <f>E80-C80</f>
-        <v>-33759.020000000004</v>
+        <v>-23160.02</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="7"/>
-      <c r="F81" s="34"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="4"/>
+      <c r="F81" s="26"/>
     </row>
     <row r="82" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="19">
+      <c r="B82" s="38"/>
+      <c r="C82" s="13">
         <f>C26-C80</f>
         <v>213.75</v>
       </c>
-      <c r="D82" s="28"/>
-      <c r="E82" s="40">
+      <c r="D82" s="20"/>
+      <c r="E82" s="32">
         <f>E26-E80</f>
-        <v>5442.77</v>
-      </c>
-      <c r="F82" s="41">
+        <v>-5156.2299999999996</v>
+      </c>
+      <c r="F82" s="33">
         <f>F26-F80</f>
-        <v>5229.0200000000041</v>
+        <v>-5369.98</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update OSI Svomming 2022 budget
</commit_message>
<xml_diff>
--- a/OSI/Budget.xlsx
+++ b/OSI/Budget.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C78B8-AD80-425F-8716-BD39F591AABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF3A3EE-4B2B-4B60-98EC-E1887A169C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,37 +581,37 @@
     <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -978,67 +978,67 @@
     <col min="5" max="5" width="14.42578125" style="23"/>
     <col min="6" max="6" width="14.42578125" style="25"/>
     <col min="7" max="7" width="14.42578125" style="1"/>
-    <col min="8" max="8" width="14.42578125" style="43"/>
+    <col min="8" max="8" width="14.42578125" style="35"/>
     <col min="9" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="43"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="43"/>
       <c r="C2" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
@@ -1059,7 +1059,7 @@
       <c r="F9" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="36" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1077,14 +1077,14 @@
       <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="34">
         <v>2990</v>
       </c>
       <c r="F10" s="26">
         <f>E10-C10</f>
         <v>-4010</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="35">
         <v>6000</v>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
         <f t="shared" ref="F14:F26" si="0">E14-C14</f>
         <v>-19300</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="35">
         <v>20800</v>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
         <f t="shared" si="0"/>
         <v>2700</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H15" s="35">
         <v>4600</v>
       </c>
     </row>
@@ -1234,14 +1234,14 @@
       <c r="D20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="34">
         <v>12880</v>
       </c>
       <c r="F20" s="26">
         <f t="shared" si="0"/>
         <v>-7920</v>
       </c>
-      <c r="H20" s="43">
+      <c r="H20" s="35">
         <v>26000</v>
       </c>
     </row>
@@ -1333,10 +1333,10 @@
       <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="40"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="15"/>
       <c r="D28" s="4"/>
       <c r="E28" s="24"/>
@@ -1390,7 +1390,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="26"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>5350</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="26"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>5990</v>
       </c>
@@ -1414,11 +1414,11 @@
       <c r="E34" s="24"/>
       <c r="F34" s="26"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="41" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="41"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="16">
         <f>SUM(C29:C34)</f>
         <v>0</v>
@@ -1427,7 +1427,7 @@
       <c r="E35" s="24"/>
       <c r="F35" s="26"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="14"/>
@@ -1435,7 +1435,7 @@
       <c r="E36" s="24"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
         <v>41</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="E37" s="24"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>4110</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>-9065</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>4120</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>7599</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>4150</v>
       </c>
@@ -1495,7 +1495,7 @@
       <c r="E40" s="24"/>
       <c r="F40" s="26"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>4200</v>
       </c>
@@ -1518,8 +1518,11 @@
       <c r="G41" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="35">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>4300</v>
       </c>
@@ -1531,7 +1534,7 @@
       <c r="E42" s="24"/>
       <c r="F42" s="26"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>4500</v>
       </c>
@@ -1543,7 +1546,7 @@
       <c r="E43" s="24"/>
       <c r="F43" s="26"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>4510</v>
       </c>
@@ -1555,7 +1558,7 @@
       <c r="E44" s="24"/>
       <c r="F44" s="26"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>4610</v>
       </c>
@@ -1567,7 +1570,7 @@
       <c r="E45" s="24"/>
       <c r="F45" s="26"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>4700</v>
       </c>
@@ -1579,7 +1582,7 @@
       <c r="E46" s="24"/>
       <c r="F46" s="26"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>4800</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>4990</v>
       </c>
@@ -1622,6 +1625,9 @@
       <c r="F48" s="26">
         <f t="shared" si="1"/>
         <v>-10199.450000000001</v>
+      </c>
+      <c r="H48" s="35">
+        <v>15000</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1810,7 +1816,7 @@
         <f t="shared" si="1"/>
         <v>-85</v>
       </c>
-      <c r="H63" s="43">
+      <c r="H63" s="35">
         <v>85</v>
       </c>
     </row>
@@ -1832,7 +1838,7 @@
         <f t="shared" si="1"/>
         <v>-136.25</v>
       </c>
-      <c r="H64" s="43">
+      <c r="H64" s="35">
         <v>136.25</v>
       </c>
     </row>
@@ -1854,7 +1860,7 @@
         <f t="shared" si="1"/>
         <v>-1500</v>
       </c>
-      <c r="H65" s="43">
+      <c r="H65" s="35">
         <v>1500</v>
       </c>
     </row>
@@ -1878,8 +1884,8 @@
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="H66" s="43">
-        <v>500</v>
+      <c r="H66" s="35">
+        <v>1000</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -1900,7 +1906,7 @@
         <f t="shared" si="1"/>
         <v>-5990.07</v>
       </c>
-      <c r="H67" s="43">
+      <c r="H67" s="35">
         <v>7000</v>
       </c>
     </row>
@@ -2025,10 +2031,10 @@
       <c r="F77" s="26"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="41"/>
+      <c r="B78" s="37"/>
       <c r="C78" s="13">
         <f>SUM(C38:C77)</f>
         <v>50286.25</v>
@@ -2098,21 +2104,21 @@
     <row r="83" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Add financial document for OSI Svomming's new equipment
</commit_message>
<xml_diff>
--- a/OSI/Budget.xlsx
+++ b/OSI/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF3A3EE-4B2B-4B60-98EC-E1887A169C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B0672A-F67B-44D3-B1B6-37366265EE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,28 +590,28 @@
     <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -983,70 +983,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="44"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="41"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1306,10 +1306,10 @@
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="13">
         <f>SUM(C10:C25)</f>
         <v>50500</v>
@@ -1333,10 +1333,10 @@
       <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="42"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="15"/>
       <c r="D28" s="4"/>
       <c r="E28" s="24"/>
@@ -1415,10 +1415,10 @@
       <c r="F34" s="26"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="37"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="16">
         <f>SUM(C29:C34)</f>
         <v>0</v>
@@ -1436,10 +1436,10 @@
       <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="17"/>
       <c r="D37" s="4"/>
       <c r="E37" s="24"/>
@@ -1620,11 +1620,11 @@
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="24">
-        <v>4800.55</v>
+        <v>5044.29</v>
       </c>
       <c r="F48" s="26">
         <f t="shared" si="1"/>
-        <v>-10199.450000000001</v>
+        <v>-9955.7099999999991</v>
       </c>
       <c r="H48" s="35">
         <v>15000</v>
@@ -2031,10 +2031,10 @@
       <c r="F77" s="26"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="37"/>
+      <c r="B78" s="44"/>
       <c r="C78" s="13">
         <f>SUM(C38:C77)</f>
         <v>50286.25</v>
@@ -2042,11 +2042,11 @@
       <c r="D78" s="4"/>
       <c r="E78" s="24">
         <f>SUM(E38:E77)</f>
-        <v>27126.23</v>
+        <v>27369.97</v>
       </c>
       <c r="F78" s="26">
         <f t="shared" si="1"/>
-        <v>-23160.02</v>
+        <v>-22916.28</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2057,10 +2057,10 @@
       <c r="F79" s="26"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="39"/>
+      <c r="B80" s="42"/>
       <c r="C80" s="13">
         <f>C78+C35</f>
         <v>50286.25</v>
@@ -2068,11 +2068,11 @@
       <c r="D80" s="4"/>
       <c r="E80" s="31">
         <f>E78</f>
-        <v>27126.23</v>
+        <v>27369.97</v>
       </c>
       <c r="F80" s="30">
         <f>E80-C80</f>
-        <v>-23160.02</v>
+        <v>-22916.28</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2083,10 +2083,10 @@
       <c r="F81" s="26"/>
     </row>
     <row r="82" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="38" t="s">
+      <c r="A82" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="38"/>
+      <c r="B82" s="41"/>
       <c r="C82" s="13">
         <f>C26-C80</f>
         <v>213.75</v>
@@ -2094,31 +2094,31 @@
       <c r="D82" s="20"/>
       <c r="E82" s="32">
         <f>E26-E80</f>
-        <v>-5156.2299999999996</v>
+        <v>-5399.9700000000012</v>
       </c>
       <c r="F82" s="33">
         <f>F26-F80</f>
-        <v>-5369.98</v>
+        <v>-5613.7200000000012</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update OSI Svomming's 2022 budget
</commit_message>
<xml_diff>
--- a/OSI/Budget.xlsx
+++ b/OSI/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B0672A-F67B-44D3-B1B6-37366265EE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14D834B-D061-446E-AF15-912E93DE3D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
     <numFmt numFmtId="166" formatCode="[$kr-414]\ #,##0.00"/>
     <numFmt numFmtId="167" formatCode="_-[$kr-414]\ * #,##0.00_-;\-[$kr-414]\ * #,##0.00_-;_-[$kr-414]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -383,6 +383,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2C3E50"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -480,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -590,29 +596,38 @@
     <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -965,88 +980,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="23"/>
-    <col min="6" max="6" width="14.42578125" style="25"/>
-    <col min="7" max="7" width="14.42578125" style="1"/>
-    <col min="8" max="8" width="14.42578125" style="35"/>
-    <col min="9" max="16384" width="14.42578125" style="1"/>
+    <col min="5" max="5" width="14.44140625" style="23"/>
+    <col min="6" max="6" width="14.44140625" style="25"/>
+    <col min="7" max="7" width="14.44140625" style="1"/>
+    <col min="8" max="8" width="14.44140625" style="35"/>
+    <col min="9" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1063,7 +1078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>3110</v>
       </c>
@@ -1088,7 +1103,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3120</v>
       </c>
@@ -1100,7 +1115,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>3400</v>
       </c>
@@ -1112,7 +1127,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>3440</v>
       </c>
@@ -1124,7 +1139,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>3480</v>
       </c>
@@ -1144,10 +1159,11 @@
         <v>-19300</v>
       </c>
       <c r="H14" s="35">
-        <v>20800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f>H20</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>3490</v>
       </c>
@@ -1172,7 +1188,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>3610</v>
       </c>
@@ -1184,7 +1200,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>3630</v>
       </c>
@@ -1196,7 +1212,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>3900</v>
       </c>
@@ -1208,7 +1224,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>3910</v>
       </c>
@@ -1220,7 +1236,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="26"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>3920</v>
       </c>
@@ -1245,7 +1261,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>3940</v>
       </c>
@@ -1257,7 +1273,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3950</v>
       </c>
@@ -1269,7 +1285,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3960</v>
       </c>
@@ -1281,7 +1297,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>3970</v>
       </c>
@@ -1293,7 +1309,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="26"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>3990</v>
       </c>
@@ -1305,11 +1321,11 @@
       <c r="E25" s="24"/>
       <c r="F25" s="26"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="42"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="13">
         <f>SUM(C10:C25)</f>
         <v>50500</v>
@@ -1323,8 +1339,12 @@
         <f t="shared" si="0"/>
         <v>-28530</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H26" s="37">
+        <f>SUM(H10:H25)</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="14"/>
@@ -1332,17 +1352,17 @@
       <c r="E27" s="24"/>
       <c r="F27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="43" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="43"/>
+      <c r="B28" s="44"/>
       <c r="C28" s="15"/>
       <c r="D28" s="4"/>
       <c r="E28" s="24"/>
       <c r="F28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>5010</v>
       </c>
@@ -1354,7 +1374,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>5011</v>
       </c>
@@ -1366,7 +1386,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="26"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>5020</v>
       </c>
@@ -1378,7 +1398,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="26"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>5250</v>
       </c>
@@ -1390,7 +1410,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="26"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>5350</v>
       </c>
@@ -1402,7 +1422,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="26"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>5990</v>
       </c>
@@ -1414,11 +1434,11 @@
       <c r="E34" s="24"/>
       <c r="F34" s="26"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="44" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="44"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="16">
         <f>SUM(C29:C34)</f>
         <v>0</v>
@@ -1426,8 +1446,12 @@
       <c r="D35" s="4"/>
       <c r="E35" s="24"/>
       <c r="F35" s="26"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="37">
+        <f>SUM(H29:H34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="14"/>
@@ -1435,17 +1459,17 @@
       <c r="E36" s="24"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="41" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="41"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="17"/>
       <c r="D37" s="4"/>
       <c r="E37" s="24"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4110</v>
       </c>
@@ -1463,8 +1487,11 @@
         <f>E38-C38</f>
         <v>-9065</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="35">
+        <v>9065</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>4120</v>
       </c>
@@ -1476,14 +1503,17 @@
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="24">
-        <v>10599</v>
+        <v>9338.7099999999991</v>
       </c>
       <c r="F39" s="26">
         <f>E39-C39</f>
-        <v>7599</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6338.7099999999991</v>
+      </c>
+      <c r="H39" s="35">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>4150</v>
       </c>
@@ -1495,7 +1525,7 @@
       <c r="E40" s="24"/>
       <c r="F40" s="26"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>4200</v>
       </c>
@@ -1522,7 +1552,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>4300</v>
       </c>
@@ -1534,7 +1564,7 @@
       <c r="E42" s="24"/>
       <c r="F42" s="26"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>4500</v>
       </c>
@@ -1546,7 +1576,7 @@
       <c r="E43" s="24"/>
       <c r="F43" s="26"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>4510</v>
       </c>
@@ -1558,7 +1588,7 @@
       <c r="E44" s="24"/>
       <c r="F44" s="26"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>4610</v>
       </c>
@@ -1570,7 +1600,7 @@
       <c r="E45" s="24"/>
       <c r="F45" s="26"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>4700</v>
       </c>
@@ -1582,7 +1612,7 @@
       <c r="E46" s="24"/>
       <c r="F46" s="26"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>4800</v>
       </c>
@@ -1607,7 +1637,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>4990</v>
       </c>
@@ -1620,17 +1650,17 @@
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="24">
-        <v>5044.29</v>
+        <v>5324.29</v>
       </c>
       <c r="F48" s="26">
         <f t="shared" si="1"/>
-        <v>-9955.7099999999991</v>
+        <v>-9675.7099999999991</v>
       </c>
       <c r="H48" s="35">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>6110</v>
       </c>
@@ -1642,7 +1672,7 @@
       <c r="E49" s="24"/>
       <c r="F49" s="26"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>6300</v>
       </c>
@@ -1654,7 +1684,7 @@
       <c r="E50" s="24"/>
       <c r="F50" s="26"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>6320</v>
       </c>
@@ -1666,7 +1696,7 @@
       <c r="E51" s="24"/>
       <c r="F51" s="26"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>6340</v>
       </c>
@@ -1678,7 +1708,7 @@
       <c r="E52" s="24"/>
       <c r="F52" s="26"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>6420</v>
       </c>
@@ -1690,7 +1720,7 @@
       <c r="E53" s="24"/>
       <c r="F53" s="26"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>6440</v>
       </c>
@@ -1702,7 +1732,7 @@
       <c r="E54" s="24"/>
       <c r="F54" s="26"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>6540</v>
       </c>
@@ -1714,7 +1744,7 @@
       <c r="E55" s="24"/>
       <c r="F55" s="26"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>6550</v>
       </c>
@@ -1726,7 +1756,7 @@
       <c r="E56" s="24"/>
       <c r="F56" s="26"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>6620</v>
       </c>
@@ -1738,7 +1768,7 @@
       <c r="E57" s="24"/>
       <c r="F57" s="26"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>6700</v>
       </c>
@@ -1750,7 +1780,7 @@
       <c r="E58" s="24"/>
       <c r="F58" s="26"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>6712</v>
       </c>
@@ -1762,7 +1792,7 @@
       <c r="E59" s="24"/>
       <c r="F59" s="26"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>6730</v>
       </c>
@@ -1774,7 +1804,7 @@
       <c r="E60" s="24"/>
       <c r="F60" s="26"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>6790</v>
       </c>
@@ -1786,7 +1816,7 @@
       <c r="E61" s="24"/>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>6800</v>
       </c>
@@ -1798,7 +1828,7 @@
       <c r="E62" s="24"/>
       <c r="F62" s="26"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>6810</v>
       </c>
@@ -1820,7 +1850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>6811</v>
       </c>
@@ -1842,7 +1872,7 @@
         <v>136.25</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>6820</v>
       </c>
@@ -1854,17 +1884,17 @@
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="24">
-        <v>0</v>
+        <v>2532</v>
       </c>
       <c r="F65" s="26">
         <f t="shared" si="1"/>
-        <v>-1500</v>
+        <v>1032</v>
       </c>
       <c r="H65" s="35">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>6840</v>
       </c>
@@ -1888,7 +1918,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>6860</v>
       </c>
@@ -1900,17 +1930,17 @@
       </c>
       <c r="D67" s="20"/>
       <c r="E67" s="24">
-        <v>1009.93</v>
+        <v>2509.9299999999998</v>
       </c>
       <c r="F67" s="26">
         <f t="shared" si="1"/>
-        <v>-5990.07</v>
+        <v>-4490.07</v>
       </c>
       <c r="H67" s="35">
         <v>7000</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>6900</v>
       </c>
@@ -1922,7 +1952,7 @@
       <c r="E68" s="24"/>
       <c r="F68" s="26"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>6940</v>
       </c>
@@ -1934,7 +1964,7 @@
       <c r="E69" s="24"/>
       <c r="F69" s="26"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>7100</v>
       </c>
@@ -1946,7 +1976,7 @@
       <c r="E70" s="24"/>
       <c r="F70" s="26"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>7110</v>
       </c>
@@ -1958,7 +1988,7 @@
       <c r="E71" s="24"/>
       <c r="F71" s="26"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>7320</v>
       </c>
@@ -1970,7 +2000,7 @@
       <c r="E72" s="24"/>
       <c r="F72" s="26"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>7420</v>
       </c>
@@ -1982,7 +2012,7 @@
       <c r="E73" s="24"/>
       <c r="F73" s="26"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>7500</v>
       </c>
@@ -1994,7 +2024,7 @@
       <c r="E74" s="24"/>
       <c r="F74" s="26"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>7510</v>
       </c>
@@ -2006,7 +2036,7 @@
       <c r="E75" s="24"/>
       <c r="F75" s="26"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>7700</v>
       </c>
@@ -2018,7 +2048,7 @@
       <c r="E76" s="24"/>
       <c r="F76" s="26"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
         <v>7790</v>
       </c>
@@ -2030,37 +2060,41 @@
       <c r="E77" s="24"/>
       <c r="F77" s="26"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="44" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="44"/>
-      <c r="C78" s="13">
+      <c r="B78" s="39"/>
+      <c r="C78" s="47">
         <f>SUM(C38:C77)</f>
         <v>50286.25</v>
       </c>
       <c r="D78" s="4"/>
-      <c r="E78" s="24">
+      <c r="E78" s="29">
         <f>SUM(E38:E77)</f>
-        <v>27369.97</v>
-      </c>
-      <c r="F78" s="26">
+        <v>30421.68</v>
+      </c>
+      <c r="F78" s="30">
         <f t="shared" si="1"/>
-        <v>-22916.28</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-19864.57</v>
+      </c>
+      <c r="H78" s="37">
+        <f>SUM(H38:H77)</f>
+        <v>62286.25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
       <c r="D79" s="4"/>
       <c r="F79" s="26"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="42" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="42"/>
+      <c r="B80" s="41"/>
       <c r="C80" s="13">
         <f>C78+C35</f>
         <v>50286.25</v>
@@ -2068,25 +2102,29 @@
       <c r="D80" s="4"/>
       <c r="E80" s="31">
         <f>E78</f>
-        <v>27369.97</v>
+        <v>30421.68</v>
       </c>
       <c r="F80" s="30">
         <f>E80-C80</f>
-        <v>-22916.28</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-19864.57</v>
+      </c>
+      <c r="H80" s="37">
+        <f>H35+H78</f>
+        <v>62286.25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
       <c r="D81" s="4"/>
       <c r="F81" s="26"/>
     </row>
-    <row r="82" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="41" t="s">
+    <row r="82" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="41"/>
+      <c r="B82" s="40"/>
       <c r="C82" s="13">
         <f>C26-C80</f>
         <v>213.75</v>
@@ -2094,31 +2132,35 @@
       <c r="D82" s="20"/>
       <c r="E82" s="32">
         <f>E26-E80</f>
-        <v>-5399.9700000000012</v>
+        <v>-8451.68</v>
       </c>
       <c r="F82" s="33">
         <f>F26-F80</f>
-        <v>-5613.7200000000012</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+        <v>-8665.43</v>
+      </c>
+      <c r="H82" s="38">
+        <f>H26-H80</f>
+        <v>313.75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Add Board dinner receipt
</commit_message>
<xml_diff>
--- a/OSI/Budget.xlsx
+++ b/OSI/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14D834B-D061-446E-AF15-912E93DE3D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05C050A-43CA-4C26-9FE5-D88201D2F57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="21270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,23 +602,8 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -626,8 +611,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,59 +981,59 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="23"/>
-    <col min="6" max="6" width="14.44140625" style="25"/>
-    <col min="7" max="7" width="14.44140625" style="1"/>
-    <col min="8" max="8" width="14.44140625" style="35"/>
-    <col min="9" max="16384" width="14.44140625" style="1"/>
+    <col min="5" max="5" width="14.42578125" style="23"/>
+    <col min="6" max="6" width="14.42578125" style="25"/>
+    <col min="7" max="7" width="14.42578125" style="1"/>
+    <col min="8" max="8" width="14.42578125" style="35"/>
+    <col min="9" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="45"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1049,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="43" t="s">
         <v>9</v>
       </c>
@@ -1057,11 +1057,11 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="40"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>3110</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>3120</v>
       </c>
@@ -1115,7 +1115,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>3400</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>3440</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>3480</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>3490</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>3610</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>3630</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>3900</v>
       </c>
@@ -1224,7 +1224,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>3910</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="26"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>3920</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>3940</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>3950</v>
       </c>
@@ -1285,7 +1285,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>3960</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>3970</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="26"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>3990</v>
       </c>
@@ -1321,11 +1321,11 @@
       <c r="E25" s="24"/>
       <c r="F25" s="26"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="41"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="13">
         <f>SUM(C10:C25)</f>
         <v>50500</v>
@@ -1344,7 +1344,7 @@
         <v>62600</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="14"/>
@@ -1352,17 +1352,17 @@
       <c r="E27" s="24"/>
       <c r="F27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="44"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="15"/>
       <c r="D28" s="4"/>
       <c r="E28" s="24"/>
       <c r="F28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>5010</v>
       </c>
@@ -1374,7 +1374,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>5011</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="26"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>5020</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="26"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>5250</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="26"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>5350</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="26"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>5990</v>
       </c>
@@ -1434,11 +1434,11 @@
       <c r="E34" s="24"/>
       <c r="F34" s="26"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="16">
         <f>SUM(C29:C34)</f>
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="14"/>
@@ -1459,17 +1459,17 @@
       <c r="E36" s="24"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="40"/>
+      <c r="B37" s="44"/>
       <c r="C37" s="17"/>
       <c r="D37" s="4"/>
       <c r="E37" s="24"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>4110</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>9065</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>4120</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>4150</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="E40" s="24"/>
       <c r="F40" s="26"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>4200</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>4300</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="E42" s="24"/>
       <c r="F42" s="26"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>4500</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="E43" s="24"/>
       <c r="F43" s="26"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>4510</v>
       </c>
@@ -1588,7 +1588,7 @@
       <c r="E44" s="24"/>
       <c r="F44" s="26"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>4610</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="E45" s="24"/>
       <c r="F45" s="26"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>4700</v>
       </c>
@@ -1612,7 +1612,7 @@
       <c r="E46" s="24"/>
       <c r="F46" s="26"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>4800</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>4990</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>6110</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="E49" s="24"/>
       <c r="F49" s="26"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>6300</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="E50" s="24"/>
       <c r="F50" s="26"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>6320</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="E51" s="24"/>
       <c r="F51" s="26"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>6340</v>
       </c>
@@ -1708,7 +1708,7 @@
       <c r="E52" s="24"/>
       <c r="F52" s="26"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>6420</v>
       </c>
@@ -1720,7 +1720,7 @@
       <c r="E53" s="24"/>
       <c r="F53" s="26"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>6440</v>
       </c>
@@ -1732,7 +1732,7 @@
       <c r="E54" s="24"/>
       <c r="F54" s="26"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>6540</v>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="E55" s="24"/>
       <c r="F55" s="26"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>6550</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="E56" s="24"/>
       <c r="F56" s="26"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>6620</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="E57" s="24"/>
       <c r="F57" s="26"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>6700</v>
       </c>
@@ -1780,7 +1780,7 @@
       <c r="E58" s="24"/>
       <c r="F58" s="26"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>6712</v>
       </c>
@@ -1792,7 +1792,7 @@
       <c r="E59" s="24"/>
       <c r="F59" s="26"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>6730</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="E60" s="24"/>
       <c r="F60" s="26"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>6790</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="E61" s="24"/>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>6800</v>
       </c>
@@ -1828,7 +1828,7 @@
       <c r="E62" s="24"/>
       <c r="F62" s="26"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>6810</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>6811</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>136.25</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>6820</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>6840</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>6860</v>
       </c>
@@ -1930,17 +1930,17 @@
       </c>
       <c r="D67" s="20"/>
       <c r="E67" s="24">
-        <v>2509.9299999999998</v>
+        <v>5509.93</v>
       </c>
       <c r="F67" s="26">
         <f t="shared" si="1"/>
-        <v>-4490.07</v>
+        <v>-1490.0699999999997</v>
       </c>
       <c r="H67" s="35">
         <v>7000</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>6900</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="E68" s="24"/>
       <c r="F68" s="26"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>6940</v>
       </c>
@@ -1964,7 +1964,7 @@
       <c r="E69" s="24"/>
       <c r="F69" s="26"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>7100</v>
       </c>
@@ -1976,7 +1976,7 @@
       <c r="E70" s="24"/>
       <c r="F70" s="26"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>7110</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="E71" s="24"/>
       <c r="F71" s="26"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>7320</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="E72" s="24"/>
       <c r="F72" s="26"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>7420</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="E73" s="24"/>
       <c r="F73" s="26"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>7500</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="E74" s="24"/>
       <c r="F74" s="26"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>7510</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="E75" s="24"/>
       <c r="F75" s="26"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>7700</v>
       </c>
@@ -2048,7 +2048,7 @@
       <c r="E76" s="24"/>
       <c r="F76" s="26"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>7790</v>
       </c>
@@ -2060,41 +2060,41 @@
       <c r="E77" s="24"/>
       <c r="F77" s="26"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="39" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="47">
+      <c r="B78" s="47"/>
+      <c r="C78" s="39">
         <f>SUM(C38:C77)</f>
         <v>50286.25</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="29">
         <f>SUM(E38:E77)</f>
-        <v>30421.68</v>
+        <v>33421.68</v>
       </c>
       <c r="F78" s="30">
         <f t="shared" si="1"/>
-        <v>-19864.57</v>
+        <v>-16864.57</v>
       </c>
       <c r="H78" s="37">
         <f>SUM(H38:H77)</f>
         <v>62286.25</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
       <c r="D79" s="4"/>
       <c r="F79" s="26"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="41" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="41"/>
+      <c r="B80" s="45"/>
       <c r="C80" s="13">
         <f>C78+C35</f>
         <v>50286.25</v>
@@ -2102,29 +2102,29 @@
       <c r="D80" s="4"/>
       <c r="E80" s="31">
         <f>E78</f>
-        <v>30421.68</v>
+        <v>33421.68</v>
       </c>
       <c r="F80" s="30">
         <f>E80-C80</f>
-        <v>-19864.57</v>
+        <v>-16864.57</v>
       </c>
       <c r="H80" s="37">
         <f>H35+H78</f>
         <v>62286.25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="21"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
       <c r="D81" s="4"/>
       <c r="F81" s="26"/>
     </row>
-    <row r="82" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="40" t="s">
+    <row r="82" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="40"/>
+      <c r="B82" s="44"/>
       <c r="C82" s="13">
         <f>C26-C80</f>
         <v>213.75</v>
@@ -2132,35 +2132,35 @@
       <c r="D82" s="20"/>
       <c r="E82" s="32">
         <f>E26-E80</f>
-        <v>-8451.68</v>
+        <v>-11451.68</v>
       </c>
       <c r="F82" s="33">
         <f>F26-F80</f>
-        <v>-8665.43</v>
+        <v>-11665.43</v>
       </c>
       <c r="H82" s="38">
         <f>H26-H80</f>
         <v>313.75</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Add methodology section to GPA paper abstract
</commit_message>
<xml_diff>
--- a/OSI/Budget.xlsx
+++ b/OSI/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05C050A-43CA-4C26-9FE5-D88201D2F57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B00D50-2CBC-47F7-948D-E407F84BE0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="21270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="-5530" windowWidth="19380" windowHeight="10980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,28 +605,28 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -980,88 +980,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="23"/>
-    <col min="6" max="6" width="14.42578125" style="25"/>
-    <col min="7" max="7" width="14.42578125" style="1"/>
-    <col min="8" max="8" width="14.42578125" style="35"/>
-    <col min="9" max="16384" width="14.42578125" style="1"/>
+    <col min="5" max="5" width="14.44140625" style="23"/>
+    <col min="6" max="6" width="14.44140625" style="25"/>
+    <col min="7" max="7" width="14.44140625" style="1"/>
+    <col min="8" max="8" width="14.44140625" style="35"/>
+    <col min="9" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="42"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="43"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="44"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>3110</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3120</v>
       </c>
@@ -1115,7 +1115,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>3400</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>3440</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>3480</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>3490</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>3610</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>3630</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>3900</v>
       </c>
@@ -1224,7 +1224,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>3910</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="26"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>3920</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>3940</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3950</v>
       </c>
@@ -1285,7 +1285,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3960</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>3970</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="26"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>3990</v>
       </c>
@@ -1321,11 +1321,11 @@
       <c r="E25" s="24"/>
       <c r="F25" s="26"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="45" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="45"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="13">
         <f>SUM(C10:C25)</f>
         <v>50500</v>
@@ -1344,7 +1344,7 @@
         <v>62600</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="14"/>
@@ -1352,17 +1352,17 @@
       <c r="E27" s="24"/>
       <c r="F27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="46"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="15"/>
       <c r="D28" s="4"/>
       <c r="E28" s="24"/>
       <c r="F28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>5010</v>
       </c>
@@ -1374,7 +1374,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>5011</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="26"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>5020</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="26"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>5250</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="26"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>5350</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="26"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>5990</v>
       </c>
@@ -1434,11 +1434,11 @@
       <c r="E34" s="24"/>
       <c r="F34" s="26"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="47" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="47"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="16">
         <f>SUM(C29:C34)</f>
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="14"/>
@@ -1459,17 +1459,17 @@
       <c r="E36" s="24"/>
       <c r="F36" s="26"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="44" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="44"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="17"/>
       <c r="D37" s="4"/>
       <c r="E37" s="24"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4110</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>9065</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>4120</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>4150</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="E40" s="24"/>
       <c r="F40" s="26"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>4200</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>4300</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="E42" s="24"/>
       <c r="F42" s="26"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>4500</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="E43" s="24"/>
       <c r="F43" s="26"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>4510</v>
       </c>
@@ -1588,7 +1588,7 @@
       <c r="E44" s="24"/>
       <c r="F44" s="26"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>4610</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="E45" s="24"/>
       <c r="F45" s="26"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>4700</v>
       </c>
@@ -1612,7 +1612,7 @@
       <c r="E46" s="24"/>
       <c r="F46" s="26"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>4800</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>4990</v>
       </c>
@@ -1657,10 +1657,10 @@
         <v>-9675.7099999999991</v>
       </c>
       <c r="H48" s="35">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>6110</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="E49" s="24"/>
       <c r="F49" s="26"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>6300</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="E50" s="24"/>
       <c r="F50" s="26"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>6320</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="E51" s="24"/>
       <c r="F51" s="26"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>6340</v>
       </c>
@@ -1708,7 +1708,7 @@
       <c r="E52" s="24"/>
       <c r="F52" s="26"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>6420</v>
       </c>
@@ -1720,7 +1720,7 @@
       <c r="E53" s="24"/>
       <c r="F53" s="26"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>6440</v>
       </c>
@@ -1732,7 +1732,7 @@
       <c r="E54" s="24"/>
       <c r="F54" s="26"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>6540</v>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="E55" s="24"/>
       <c r="F55" s="26"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>6550</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="E56" s="24"/>
       <c r="F56" s="26"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>6620</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="E57" s="24"/>
       <c r="F57" s="26"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>6700</v>
       </c>
@@ -1780,7 +1780,7 @@
       <c r="E58" s="24"/>
       <c r="F58" s="26"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>6712</v>
       </c>
@@ -1792,7 +1792,7 @@
       <c r="E59" s="24"/>
       <c r="F59" s="26"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>6730</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="E60" s="24"/>
       <c r="F60" s="26"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>6790</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="E61" s="24"/>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>6800</v>
       </c>
@@ -1828,7 +1828,7 @@
       <c r="E62" s="24"/>
       <c r="F62" s="26"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>6810</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>6811</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>136.25</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>6820</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>6840</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>6860</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>6900</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="E68" s="24"/>
       <c r="F68" s="26"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>6940</v>
       </c>
@@ -1964,7 +1964,7 @@
       <c r="E69" s="24"/>
       <c r="F69" s="26"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>7100</v>
       </c>
@@ -1976,7 +1976,7 @@
       <c r="E70" s="24"/>
       <c r="F70" s="26"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>7110</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="E71" s="24"/>
       <c r="F71" s="26"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>7320</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="E72" s="24"/>
       <c r="F72" s="26"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>7420</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="E73" s="24"/>
       <c r="F73" s="26"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>7500</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="E74" s="24"/>
       <c r="F74" s="26"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>7510</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="E75" s="24"/>
       <c r="F75" s="26"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>7700</v>
       </c>
@@ -2048,7 +2048,7 @@
       <c r="E76" s="24"/>
       <c r="F76" s="26"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
         <v>7790</v>
       </c>
@@ -2060,11 +2060,11 @@
       <c r="E77" s="24"/>
       <c r="F77" s="26"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="47" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="47"/>
+      <c r="B78" s="40"/>
       <c r="C78" s="39">
         <f>SUM(C38:C77)</f>
         <v>50286.25</v>
@@ -2080,21 +2080,21 @@
       </c>
       <c r="H78" s="37">
         <f>SUM(H38:H77)</f>
-        <v>62286.25</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47286.25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
       <c r="D79" s="4"/>
       <c r="F79" s="26"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="45" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="45"/>
+      <c r="B80" s="42"/>
       <c r="C80" s="13">
         <f>C78+C35</f>
         <v>50286.25</v>
@@ -2110,21 +2110,21 @@
       </c>
       <c r="H80" s="37">
         <f>H35+H78</f>
-        <v>62286.25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47286.25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
       <c r="D81" s="4"/>
       <c r="F81" s="26"/>
     </row>
-    <row r="82" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
+    <row r="82" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="44"/>
+      <c r="B82" s="41"/>
       <c r="C82" s="13">
         <f>C26-C80</f>
         <v>213.75</v>
@@ -2140,27 +2140,27 @@
       </c>
       <c r="H82" s="38">
         <f>H26-H80</f>
-        <v>313.75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+        <v>15313.75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>